<commit_message>
new findings! using sigmoid kernel works surprisingly good with half and half data
</commit_message>
<xml_diff>
--- a/EDA_Process/C_Morlet_SVM/ASD_VS_TD.xlsx
+++ b/EDA_Process/C_Morlet_SVM/ASD_VS_TD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fengh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LabWork\ThesisProject\Music_Autism_Robot\EDA_Process\C_Morlet_SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E651E0E-6C1B-4CC9-9344-06D4EADAAC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993C89F8-3D80-4EF1-9B08-C18A1CB9D112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8553" yWindow="0" windowWidth="9100" windowHeight="9467" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c=0.1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>SVMAccuracy : 78.125</t>
   </si>
@@ -37,6 +37,69 @@
   </si>
   <si>
     <t>25  75</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Poly</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 62.5</t>
+  </si>
+  <si>
+    <t>50  50</t>
+  </si>
+  <si>
+    <t>RBF</t>
+  </si>
+  <si>
+    <t>100    0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75   25</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 68.75</t>
+  </si>
+  <si>
+    <t>75  25</t>
+  </si>
+  <si>
+    <t>38  63</t>
+  </si>
+  <si>
+    <t>c = 0.1, 16 samples vs 16 samples</t>
+  </si>
+  <si>
+    <t>c = 0.1, half and half, SVM vs MKL</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 75</t>
+  </si>
+  <si>
+    <t>MKLAccuracy : 68.75</t>
+  </si>
+  <si>
+    <t>63  38</t>
+  </si>
+  <si>
+    <t>13  88</t>
+  </si>
+  <si>
+    <t>MKLConfusionMatrix</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 50</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 87.5</t>
+  </si>
+  <si>
+    <t>88  13</t>
   </si>
 </sst>
 </file>
@@ -354,34 +417,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="18.64453125" customWidth="1"/>
+    <col min="2" max="2" width="18.1171875" customWidth="1"/>
+    <col min="3" max="3" width="17.76171875" customWidth="1"/>
+    <col min="4" max="4" width="17.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>